<commit_message>
Avance agregar campo monto pago en consulta de estudiantes y obligaciones
</commit_message>
<xml_diff>
--- a/docs/TASAS_IMPORTACION.xlsx
+++ b/docs/TASAS_IMPORTACION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\repos\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\repos\00043-DWeb-CuentasPorCobrar\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E025E6-1A9E-4DE5-9060-E71EA6C09700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7928F1-4FC2-4A29-8A14-E24D06910482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IRED" sheetId="1" r:id="rId1"/>
@@ -3943,7 +3943,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="POSGRADO"/>
@@ -4836,7 +4836,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="CEPREVI"/>
@@ -5673,7 +5673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -17805,7 +17805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB65E3B3-739E-4378-98B2-D70BC55BDBA4}">
   <dimension ref="A1:N140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>

</xml_diff>